<commit_message>
Added Kubernetes files and refatored project structure
</commit_message>
<xml_diff>
--- a/templates/Analysis spreadsheet template.xlsx
+++ b/templates/Analysis spreadsheet template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">CHROMAMON
 (Chromatographic Monitoring)</t>
@@ -54,6 +54,10 @@
   </si>
   <si>
     <t xml:space="preserve">Analysis Hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2 dissolved
+(ppm)</t>
   </si>
   <si>
     <t xml:space="preserve">CO dissolved
@@ -142,6 +146,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -162,18 +167,21 @@
       <sz val="10"/>
       <name val="NanumGothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="NanumGothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="NanumGothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -245,7 +253,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,7 +262,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -262,7 +270,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,6 +295,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,13 +379,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="21.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.13"/>
@@ -381,21 +393,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="14.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.49"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="23.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="20.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="17.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="22" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="14.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="23.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="17.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="23" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -441,16 +453,17 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="3"/>
+      <c r="Q4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="3" t="s">
+      <c r="S4" s="4"/>
+      <c r="T4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="3"/>
       <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
@@ -468,12 +481,13 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="4"/>
+      <c r="P5" s="3"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="3"/>
+      <c r="S5" s="4"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
@@ -518,10 +532,10 @@
       <c r="N6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="P6" s="8" t="s">
         <v>20</v>
       </c>
       <c r="Q6" s="7" t="s">
@@ -530,25 +544,28 @@
       <c r="R6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="S6" s="7" t="s">
         <v>23</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="U6" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="9" t="n">
         <v>43640</v>
@@ -559,59 +576,62 @@
       <c r="F7" s="10" t="n">
         <v>0.565972222222222</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="I7" s="1" t="n">
         <v>320</v>
       </c>
-      <c r="I7" s="1" t="n">
+      <c r="J7" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="J7" s="1" t="n">
+      <c r="K7" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="K7" s="1" t="n">
+      <c r="L7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="L7" s="1" t="n">
+      <c r="M7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="M7" s="1" t="n">
+      <c r="N7" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="N7" s="1" t="n">
+      <c r="O7" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="O7" s="1" t="n">
+      <c r="P7" s="1" t="n">
         <v>1.01</v>
       </c>
-      <c r="P7" s="1" t="n">
+      <c r="Q7" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="Q7" s="1" t="n">
+      <c r="R7" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="R7" s="1" t="n">
+      <c r="S7" s="1" t="n">
         <v>1.01</v>
       </c>
-      <c r="S7" s="9" t="n">
+      <c r="T7" s="9" t="n">
         <v>45272</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:E3"/>
     <mergeCell ref="A4:D5"/>
-    <mergeCell ref="E4:O5"/>
-    <mergeCell ref="P4:R5"/>
-    <mergeCell ref="S4:U5"/>
+    <mergeCell ref="E4:P5"/>
+    <mergeCell ref="Q4:S5"/>
+    <mergeCell ref="T4:V5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>